<commit_message>
removes Fixed from indices dataset
</commit_message>
<xml_diff>
--- a/src/technology/simple-electrolysis/simple-electrolysis.xlsx
+++ b/src/technology/simple-electrolysis/simple-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\simple-electrolysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC8F0DF-E1AE-4305-8C4C-F820D480B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3675932E-9633-4BA8-A633-BAEEDDC21CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="780" windowWidth="20910" windowHeight="11775" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
+    <workbookView xWindow="29970" yWindow="-6090" windowWidth="12150" windowHeight="21285" activeTab="2" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="101">
   <si>
     <t>Technology</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Rent</t>
   </si>
   <si>
     <t>Output</t>
@@ -702,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768C47FA-A48E-4158-95EE-1019738EA2E7}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1770,9 +1767,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB279C25-BB03-4F81-BF04-3441E556B5A5}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1818,16 +1817,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,13 +1837,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,16 +1851,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1869,16 +1868,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1889,13 +1888,13 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1903,13 +1902,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>63</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>
@@ -1920,33 +1919,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>64</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
         <v>65</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1964,13 +1946,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1978,46 +1960,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2041,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
         <v>58</v>
@@ -2064,7 +2046,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2073,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2084,7 +2066,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2093,7 +2075,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2104,7 +2086,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2113,7 +2095,7 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2124,7 +2106,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2133,7 +2115,7 @@
         <v>237</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2144,7 +2126,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -2153,7 +2135,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2164,7 +2146,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2184,7 +2166,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2193,7 +2175,7 @@
         <v>0.63</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2204,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -2213,7 +2195,7 @@
         <v>1000</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2224,7 +2206,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -2233,10 +2215,10 @@
         <v>1.08E-3</v>
       </c>
       <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
         <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2247,7 +2229,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -2256,10 +2238,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
         <v>96</v>
-      </c>
-      <c r="G11" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,7 +2252,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2279,7 +2261,7 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2290,7 +2272,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2299,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2310,7 +2292,7 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -2319,7 +2301,7 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2330,7 +2312,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -2339,7 +2321,7 @@
         <v>237</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2350,7 +2332,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -2359,7 +2341,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2370,7 +2352,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -2390,7 +2372,7 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2399,7 +2381,7 @@
         <v>0.63</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2410,7 +2392,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -2419,7 +2401,7 @@
         <v>1000</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2430,7 +2412,7 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -2439,10 +2421,10 @@
         <v>1.08E-3</v>
       </c>
       <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
         <v>93</v>
-      </c>
-      <c r="G20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2453,7 +2435,7 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -2462,10 +2444,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" t="s">
         <v>96</v>
-      </c>
-      <c r="G21" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2476,7 +2458,7 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2485,7 +2467,7 @@
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2496,7 +2478,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2505,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2516,7 +2498,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -2525,7 +2507,7 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2536,7 +2518,7 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2545,7 +2527,7 @@
         <v>237</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2556,7 +2538,7 @@
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -2565,7 +2547,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2576,7 +2558,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -2596,7 +2578,7 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -2605,7 +2587,7 @@
         <v>0.63</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2616,7 +2598,7 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -2625,7 +2607,7 @@
         <v>1000</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,7 +2618,7 @@
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -2645,10 +2627,10 @@
         <v>1.08E-3</v>
       </c>
       <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s">
         <v>93</v>
-      </c>
-      <c r="G30" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2659,7 +2641,7 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31">
         <v>9</v>
@@ -2668,10 +2650,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" t="s">
         <v>96</v>
-      </c>
-      <c r="G31" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2682,7 +2664,7 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2691,7 +2673,7 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2702,7 +2684,7 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2711,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,7 +2704,7 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2731,7 +2713,7 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2742,7 +2724,7 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -2751,7 +2733,7 @@
         <v>237</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2762,7 +2744,7 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -2771,7 +2753,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2782,7 +2764,7 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37">
         <v>5</v>
@@ -2802,7 +2784,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -2811,7 +2793,7 @@
         <v>0.63</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2822,7 +2804,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -2831,7 +2813,7 @@
         <v>1000</v>
       </c>
       <c r="F39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2842,7 +2824,7 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -2851,10 +2833,10 @@
         <v>1.08E-3</v>
       </c>
       <c r="F40" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" t="s">
         <v>93</v>
-      </c>
-      <c r="G40" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2865,7 +2847,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41">
         <v>9</v>
@@ -2874,10 +2856,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" t="s">
         <v>96</v>
-      </c>
-      <c r="G41" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2915,10 +2897,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
@@ -2929,7 +2911,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -2943,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -2957,13 +2939,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2971,13 +2953,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,13 +2967,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3009,16 +2991,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -3026,10 +3008,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3040,10 +3022,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -3054,10 +3036,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -3068,10 +3050,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
#144 updates electrolysis to remove scenarios
</commit_message>
<xml_diff>
--- a/src/technology/simple-electrolysis/simple-electrolysis.xlsx
+++ b/src/technology/simple-electrolysis/simple-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\simple-electrolysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3675932E-9633-4BA8-A633-BAEEDDC21CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561ABD9E-E498-4104-BDAC-1135E6BE9A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="-6090" windowWidth="12150" windowHeight="21285" activeTab="2" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
+    <workbookView xWindow="30990" yWindow="345" windowWidth="17730" windowHeight="15120" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,14 +42,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="96">
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -257,25 +254,13 @@
     <t>Electrolysis R&amp;D</t>
   </si>
   <si>
-    <t>No Electrolysis R&amp;D</t>
-  </si>
-  <si>
     <t>Low R&amp;D Spending</t>
   </si>
   <si>
-    <t>Low Electrolysis R&amp;D</t>
-  </si>
-  <si>
     <t>Medium R&amp;D Spending</t>
   </si>
   <si>
-    <t>Medium Electrolysis R&amp;D</t>
-  </si>
-  <si>
     <t>High R&amp;D Spending</t>
-  </si>
-  <si>
-    <t>High Electrolysis R&amp;D</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -699,65 +684,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768C47FA-A48E-4158-95EE-1019738EA2E7}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>19.04</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>0.95</v>
@@ -768,36 +759,36 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>279</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5">
         <v>0.85</v>
@@ -808,16 +799,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
       <c r="E6">
         <v>0.9</v>
@@ -828,16 +819,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>0.9</v>
@@ -848,162 +839,162 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>6650</v>
       </c>
       <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1">
         <v>3.3300000000000003E-5</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1">
         <v>0.01</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
       </c>
       <c r="E14">
         <v>19.04</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1011,39 +1002,39 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>279</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1051,19 +1042,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1071,19 +1062,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1091,162 +1082,162 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
         <v>20</v>
-      </c>
-      <c r="G20" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>6650</v>
       </c>
       <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
         <v>23</v>
-      </c>
-      <c r="G21" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1">
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1">
         <v>3.3300000000000003E-5</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="1">
         <v>0.01</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
         <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
       </c>
       <c r="E26">
         <v>19.04</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>36</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1254,39 +1245,39 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28">
         <v>279</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1294,19 +1285,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
-        <v>16</v>
-      </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1314,19 +1305,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1334,162 +1325,162 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
         <v>18</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
         <v>20</v>
-      </c>
-      <c r="G32" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33">
         <v>6650</v>
       </c>
       <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
         <v>23</v>
-      </c>
-      <c r="G33" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1">
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1">
         <v>3.3300000000000003E-5</v>
       </c>
       <c r="F35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1">
         <v>0.01</v>
       </c>
       <c r="F37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
         <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
       </c>
       <c r="E38">
         <v>19.04</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
         <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="s">
-        <v>41</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1497,39 +1488,39 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E40">
         <v>279</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
       <c r="E41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1537,19 +1528,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1557,19 +1548,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1577,125 +1568,125 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
         <v>18</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s">
         <v>20</v>
-      </c>
-      <c r="G44" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E45">
         <v>6650</v>
       </c>
       <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
         <v>23</v>
-      </c>
-      <c r="G45" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" s="1">
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E47" s="1">
         <v>3.3300000000000003E-5</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="1">
         <v>0.01</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1716,48 +1707,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1769,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB279C25-BB03-4F81-BF04-3441E556B5A5}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,155 +1771,155 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1940,66 +1931,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8DDB52-2793-4513-A7DB-EE354AA78557}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
-        <v>68</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D60756-8727-469C-BF07-9640ADCA9D3D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2020,33 +2021,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2055,18 +2056,18 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2075,18 +2076,18 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2095,18 +2096,18 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2115,18 +2116,18 @@
         <v>237</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -2135,18 +2136,18 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2155,18 +2156,18 @@
         <v>6650</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2175,18 +2176,18 @@
         <v>0.63</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -2195,18 +2196,18 @@
         <v>1000</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -2215,21 +2216,21 @@
         <v>1.08E-3</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -2238,21 +2239,21 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2261,18 +2262,18 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2281,18 +2282,18 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -2301,18 +2302,18 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -2321,18 +2322,18 @@
         <v>237</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -2341,18 +2342,18 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -2361,18 +2362,18 @@
         <v>6650</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2381,18 +2382,18 @@
         <v>0.63</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -2401,18 +2402,18 @@
         <v>1000</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -2421,21 +2422,21 @@
         <v>1.08E-3</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -2444,21 +2445,21 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2467,18 +2468,18 @@
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2487,18 +2488,18 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -2507,18 +2508,18 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2527,18 +2528,18 @@
         <v>237</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -2547,18 +2548,18 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -2567,18 +2568,18 @@
         <v>6650</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -2587,18 +2588,18 @@
         <v>0.63</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -2607,18 +2608,18 @@
         <v>1000</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -2627,21 +2628,21 @@
         <v>1.08E-3</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>9</v>
@@ -2650,21 +2651,21 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F31" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2673,18 +2674,18 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2693,18 +2694,18 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2713,18 +2714,18 @@
         <v>18.079999999999998</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -2733,18 +2734,18 @@
         <v>237</v>
       </c>
       <c r="F35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -2753,18 +2754,18 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D37">
         <v>5</v>
@@ -2773,18 +2774,18 @@
         <v>6650</v>
       </c>
       <c r="F37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -2793,18 +2794,18 @@
         <v>0.63</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -2813,18 +2814,18 @@
         <v>1000</v>
       </c>
       <c r="F39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -2833,21 +2834,21 @@
         <v>1.08E-3</v>
       </c>
       <c r="F40" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D41">
         <v>9</v>
@@ -2856,10 +2857,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G41" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2880,100 +2881,100 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2983,82 +2984,73 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6483DD-2255-49BA-BAE9-23EDEC3285E4}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
+        <v>29</v>
+      </c>
+      <c r="C3">
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
+        <v>34</v>
+      </c>
+      <c r="C4">
         <v>2500000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5">
+        <v>39</v>
+      </c>
+      <c r="C5">
         <v>5000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to the Tyche-GUI-front
</commit_message>
<xml_diff>
--- a/src/technology/simple-electrolysis/simple-electrolysis.xlsx
+++ b/src/technology/simple-electrolysis/simple-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\simple-electrolysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/tyche/src/technology/simple-electrolysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561ABD9E-E498-4104-BDAC-1135E6BE9A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{561ABD9E-E498-4104-BDAC-1135E6BE9A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07466E35-0504-9C46-9507-1517573DEB37}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="345" windowWidth="17730" windowHeight="15120" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
+    <workbookView xWindow="16820" yWindow="760" windowWidth="17740" windowHeight="15120" activeTab="4" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -684,17 +684,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768C47FA-A48E-4158-95EE-1019738EA2E7}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -737,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -777,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -860,7 +860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -880,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -900,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -920,7 +920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -940,7 +940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -960,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -980,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1700,9 +1700,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1764,9 +1764,9 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1935,15 +1935,15 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -2010,13 +2010,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D60756-8727-469C-BF07-9640ADCA9D3D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2099,7 +2103,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2123,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2159,7 +2163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2179,7 +2183,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2199,7 +2203,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2222,7 +2226,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2285,7 +2289,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -2305,7 +2309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2325,7 +2329,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2365,7 +2369,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -2405,7 +2409,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -2428,7 +2432,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -2451,7 +2455,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -2471,7 +2475,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2531,7 +2535,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2551,7 +2555,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -2591,7 +2595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -2634,7 +2638,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -2657,7 +2661,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -2697,7 +2701,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2717,7 +2721,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2757,7 +2761,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2777,7 +2781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2801,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2817,7 +2821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2840,7 +2844,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2874,9 +2878,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2907,7 +2911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2921,7 +2925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2949,7 +2953,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2963,7 +2967,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2987,16 +2991,16 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3010,7 +3014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -3021,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -3043,7 +3047,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>

</xml_diff>